<commit_message>
Update usa and twn emissions (#264)
* Update inventory data for usa and Taiwan. Update Taiwan scaling mapping.
* Adjust IEA energy to have complete time series for off-road diesel consumption
* USA and CAN offroad EFs
* Add species specific scaling mapping for USA to deal with misc emissions tier1 category.
Co-authored-by: Patrick O'Rourke <patrick.orourke@pnnl.gov>
</commit_message>
<xml_diff>
--- a/input/mappings/SO2_control_frac_last_inv_year.xlsx
+++ b/input/mappings/SO2_control_frac_last_inv_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Documents/Information &amp; Documents/CEDS_Project/CEDS/input/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486D7C36-1A17-2348-B5AC-083A5FD530B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8229E4-F108-6049-A047-3B2B9380AF9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2240" windowWidth="16720" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1187,7 +1187,7 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1805,7 +1805,7 @@
         <v>5</v>
       </c>
       <c r="B72" s="18">
-        <v>2010</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1821,7 +1821,7 @@
         <v>6</v>
       </c>
       <c r="B74" s="18">
-        <v>2014</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Canada inventory 3 (#266)
* New Canada data to 2018 with detailed sectors
* Update module E and F scripts
* Update CAN inventory mapping files. Separate scaling for NOx so that Agriculture NOx is included
* Remove previous newer can inventory
* Update can last inv year for SO2

Co-authored-by: andrea.mott@pnnl.gov <andrea.mott@pnnl.gov>
</commit_message>
<xml_diff>
--- a/input/mappings/SO2_control_frac_last_inv_year.xlsx
+++ b/input/mappings/SO2_control_frac_last_inv_year.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Documents/Information &amp; Documents/CEDS_Project/CEDS/input/mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8229E4-F108-6049-A047-3B2B9380AF9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E58459A-93EE-AF48-BE66-855E92552B64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2240" windowWidth="16720" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1186,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1307,7 +1307,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="19">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="D14" s="19"/>
     </row>

</xml_diff>